<commit_message>
[Maintain_Booking] : Chage in sheet
</commit_message>
<xml_diff>
--- a/InputData/BookingData.xlsx
+++ b/InputData/BookingData.xlsx
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="1128">
   <si>
     <t>ID</t>
   </si>
@@ -3732,21 +3732,6 @@
     <t>21-Jun-2023</t>
   </si>
   <si>
-    <t>890-363-6027</t>
-  </si>
-  <si>
-    <t>232-364-9631</t>
-  </si>
-  <si>
-    <t>232-365-2587</t>
-  </si>
-  <si>
-    <t>458-366-3654</t>
-  </si>
-  <si>
-    <t>258-367-3657</t>
-  </si>
-  <si>
     <t>125-368-2568</t>
   </si>
   <si>
@@ -3762,24 +3747,6 @@
     <t>232-372-956</t>
   </si>
   <si>
-    <t>25044</t>
-  </si>
-  <si>
-    <t>43045</t>
-  </si>
-  <si>
-    <t>42646</t>
-  </si>
-  <si>
-    <t>477147</t>
-  </si>
-  <si>
-    <t>457548</t>
-  </si>
-  <si>
-    <t>426549</t>
-  </si>
-  <si>
     <t>4523850</t>
   </si>
   <si>
@@ -3801,24 +3768,6 @@
     <t>451856</t>
   </si>
   <si>
-    <t>820043</t>
-  </si>
-  <si>
-    <t>180044</t>
-  </si>
-  <si>
-    <t>535345</t>
-  </si>
-  <si>
-    <t>166246</t>
-  </si>
-  <si>
-    <t>1HG847</t>
-  </si>
-  <si>
-    <t>1267948</t>
-  </si>
-  <si>
     <t>AAS1249</t>
   </si>
   <si>
@@ -3843,24 +3792,6 @@
     <t>BB30056</t>
   </si>
   <si>
-    <t>ICICI0000885</t>
-  </si>
-  <si>
-    <t>ICICI0000886</t>
-  </si>
-  <si>
-    <t>ICICI0000887</t>
-  </si>
-  <si>
-    <t>ICICI0000688</t>
-  </si>
-  <si>
-    <t>ICICI00063589</t>
-  </si>
-  <si>
-    <t>ICICI00072390</t>
-  </si>
-  <si>
     <t>ICICI00066791</t>
   </si>
   <si>
@@ -3882,24 +3813,6 @@
     <t>ICICI0008898</t>
   </si>
   <si>
-    <t>833801</t>
-  </si>
-  <si>
-    <t>353402</t>
-  </si>
-  <si>
-    <t>345803</t>
-  </si>
-  <si>
-    <t>324604</t>
-  </si>
-  <si>
-    <t>323505</t>
-  </si>
-  <si>
-    <t>396706</t>
-  </si>
-  <si>
     <t>353307</t>
   </si>
   <si>
@@ -3924,33 +3837,6 @@
     <t>3463514</t>
   </si>
   <si>
-    <t>PF/RD/663/2023</t>
-  </si>
-  <si>
-    <t>PF/HE/664/2023</t>
-  </si>
-  <si>
-    <t>PF/SA/665/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/666/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/667/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/6682023</t>
-  </si>
-  <si>
-    <t>PF/PR/669/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/670/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/671/2023</t>
-  </si>
-  <si>
     <t>PF/PR/672/2023</t>
   </si>
   <si>
@@ -3966,22 +3852,121 @@
     <t>PF/AP/676/2023</t>
   </si>
   <si>
-    <t>CHN/BKG/AFE/00174/23-24</t>
-  </si>
-  <si>
-    <t>MUM/BKG/AEC/00012/2122-49</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFI/00175/23-24</t>
-  </si>
-  <si>
-    <t>MUM/BKG/AFIC/00014/2122-14</t>
-  </si>
-  <si>
-    <t>MUM/BKG/CS/00033/23-24</t>
-  </si>
-  <si>
-    <t>MUM/BKG/ITCT/00034/23-24</t>
+    <t>232-372-2587</t>
+  </si>
+  <si>
+    <t>458-373-3654</t>
+  </si>
+  <si>
+    <t>258-374-3657</t>
+  </si>
+  <si>
+    <t>42652</t>
+  </si>
+  <si>
+    <t>477153</t>
+  </si>
+  <si>
+    <t>457554</t>
+  </si>
+  <si>
+    <t>426555</t>
+  </si>
+  <si>
+    <t>535352</t>
+  </si>
+  <si>
+    <t>166253</t>
+  </si>
+  <si>
+    <t>1HG854</t>
+  </si>
+  <si>
+    <t>1267955</t>
+  </si>
+  <si>
+    <t>ICICI0000892</t>
+  </si>
+  <si>
+    <t>ICICI0000693</t>
+  </si>
+  <si>
+    <t>ICICI00063594</t>
+  </si>
+  <si>
+    <t>ICICI00072395</t>
+  </si>
+  <si>
+    <t>345808</t>
+  </si>
+  <si>
+    <t>324609</t>
+  </si>
+  <si>
+    <t>323510</t>
+  </si>
+  <si>
+    <t>396711</t>
+  </si>
+  <si>
+    <t>PF/PR/673/2023</t>
+  </si>
+  <si>
+    <t>PF/SA/672/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/674/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/675/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/676/2023</t>
+  </si>
+  <si>
+    <t>890-374-6027</t>
+  </si>
+  <si>
+    <t>232-375-9631</t>
+  </si>
+  <si>
+    <t>29-Jun-2023</t>
+  </si>
+  <si>
+    <t>25054</t>
+  </si>
+  <si>
+    <t>43055</t>
+  </si>
+  <si>
+    <t>820054</t>
+  </si>
+  <si>
+    <t>180055</t>
+  </si>
+  <si>
+    <t>ICICI0000894</t>
+  </si>
+  <si>
+    <t>ICICI0000895</t>
+  </si>
+  <si>
+    <t>833808</t>
+  </si>
+  <si>
+    <t>353409</t>
+  </si>
+  <si>
+    <t>PF/RD/674/2023</t>
+  </si>
+  <si>
+    <t>PF/HE/675/2023</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00179/23-24</t>
+  </si>
+  <si>
+    <t>MUM/BKG/AEC/00012/2122-51</t>
   </si>
 </sst>
 </file>
@@ -7465,7 +7450,7 @@
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8247,30 +8232,30 @@
         <v>1</v>
       </c>
       <c r="D8" s="717" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E8" s="215" t="s">
         <v>391</v>
       </c>
       <c r="F8" s="394" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="G8" s="216"/>
       <c r="H8" s="399"/>
       <c r="I8" s="451" t="s">
-        <v>1049</v>
+        <v>1113</v>
       </c>
       <c r="J8" s="219" t="s">
         <v>393</v>
       </c>
       <c r="K8" s="403" t="s">
-        <v>1045</v>
+        <v>1115</v>
       </c>
       <c r="L8" s="404" t="s">
         <v>394</v>
       </c>
       <c r="M8" s="451" t="s">
-        <v>1059</v>
+        <v>1116</v>
       </c>
       <c r="N8" s="220" t="s">
         <v>562</v>
@@ -8282,7 +8267,7 @@
         <v>409</v>
       </c>
       <c r="Q8" s="451" t="s">
-        <v>1072</v>
+        <v>1118</v>
       </c>
       <c r="R8" s="465" t="s">
         <v>727</v>
@@ -8294,7 +8279,7 @@
         <v>562</v>
       </c>
       <c r="U8" s="426" t="s">
-        <v>1086</v>
+        <v>1120</v>
       </c>
       <c r="V8" s="425" t="s">
         <v>854</v>
@@ -8306,7 +8291,7 @@
         <v>396</v>
       </c>
       <c r="Y8" s="434" t="s">
-        <v>1099</v>
+        <v>1122</v>
       </c>
       <c r="Z8" s="435" t="s">
         <v>397</v>
@@ -8321,7 +8306,7 @@
         <v>561</v>
       </c>
       <c r="AD8" s="450" t="s">
-        <v>1113</v>
+        <v>1124</v>
       </c>
       <c r="AE8" s="452"/>
       <c r="AF8" s="451" t="s">
@@ -8415,20 +8400,20 @@
         <v>410</v>
       </c>
       <c r="D9" s="714" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E9" s="122" t="s">
         <v>391</v>
       </c>
       <c r="F9" s="396" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="G9" s="289"/>
       <c r="H9" s="401" t="s">
         <v>574</v>
       </c>
       <c r="I9" s="398" t="s">
-        <v>1050</v>
+        <v>1114</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>393</v>
@@ -8440,7 +8425,7 @@
         <v>394</v>
       </c>
       <c r="M9" s="411" t="s">
-        <v>1060</v>
+        <v>1117</v>
       </c>
       <c r="N9" s="291" t="s">
         <v>562</v>
@@ -8452,7 +8437,7 @@
         <v>409</v>
       </c>
       <c r="Q9" s="411" t="s">
-        <v>1073</v>
+        <v>1119</v>
       </c>
       <c r="R9" s="421" t="s">
         <v>395</v>
@@ -8464,7 +8449,7 @@
         <v>562</v>
       </c>
       <c r="U9" s="429" t="s">
-        <v>1087</v>
+        <v>1121</v>
       </c>
       <c r="V9" s="423" t="s">
         <v>847</v>
@@ -8474,7 +8459,7 @@
         <v>396</v>
       </c>
       <c r="Y9" s="439" t="s">
-        <v>1100</v>
+        <v>1123</v>
       </c>
       <c r="Z9" s="440" t="s">
         <v>397</v>
@@ -8487,7 +8472,7 @@
       </c>
       <c r="AC9" s="459"/>
       <c r="AD9" s="448" t="s">
-        <v>1114</v>
+        <v>1125</v>
       </c>
       <c r="AE9" s="458"/>
       <c r="AF9" s="460" t="s">
@@ -8580,19 +8565,17 @@
       <c r="C10" s="276" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="715" t="s">
-        <v>1129</v>
-      </c>
+      <c r="D10" s="715"/>
       <c r="E10" s="123" t="s">
         <v>391</v>
       </c>
       <c r="F10" s="395" t="s">
-        <v>1048</v>
+        <v>753</v>
       </c>
       <c r="G10" s="277"/>
       <c r="H10" s="400"/>
       <c r="I10" s="397" t="s">
-        <v>1051</v>
+        <v>1089</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>393</v>
@@ -8604,7 +8587,7 @@
         <v>394</v>
       </c>
       <c r="M10" s="412" t="s">
-        <v>1061</v>
+        <v>1092</v>
       </c>
       <c r="N10" s="279" t="s">
         <v>562</v>
@@ -8616,7 +8599,7 @@
         <v>409</v>
       </c>
       <c r="Q10" s="412" t="s">
-        <v>1074</v>
+        <v>1096</v>
       </c>
       <c r="R10" s="422" t="s">
         <v>395</v>
@@ -8628,7 +8611,7 @@
         <v>562</v>
       </c>
       <c r="U10" s="428" t="s">
-        <v>1088</v>
+        <v>1100</v>
       </c>
       <c r="V10" s="424" t="s">
         <v>848</v>
@@ -8640,7 +8623,7 @@
         <v>396</v>
       </c>
       <c r="Y10" s="436" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="Z10" s="437" t="s">
         <v>397</v>
@@ -8655,7 +8638,7 @@
         <v>1025</v>
       </c>
       <c r="AD10" s="449" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
       <c r="AE10" s="454"/>
       <c r="AF10" s="456" t="s">
@@ -8740,14 +8723,12 @@
       <c r="C11" s="97" t="s">
         <v>411</v>
       </c>
-      <c r="D11" s="632" t="s">
-        <v>1130</v>
-      </c>
+      <c r="D11" s="632"/>
       <c r="E11" s="90" t="s">
         <v>391</v>
       </c>
       <c r="F11" s="410" t="s">
-        <v>1048</v>
+        <v>753</v>
       </c>
       <c r="G11" s="461"/>
       <c r="H11" s="472" t="s">
@@ -8762,7 +8743,7 @@
         <v>394</v>
       </c>
       <c r="M11" s="409" t="s">
-        <v>1062</v>
+        <v>1093</v>
       </c>
       <c r="N11" s="446" t="s">
         <v>562</v>
@@ -8774,7 +8755,7 @@
         <v>409</v>
       </c>
       <c r="Q11" s="409" t="s">
-        <v>1075</v>
+        <v>1097</v>
       </c>
       <c r="R11" s="419" t="s">
         <v>395</v>
@@ -8786,7 +8767,7 @@
         <v>562</v>
       </c>
       <c r="U11" s="420" t="s">
-        <v>1089</v>
+        <v>1101</v>
       </c>
       <c r="V11" s="442" t="s">
         <v>849</v>
@@ -8796,7 +8777,7 @@
         <v>396</v>
       </c>
       <c r="Y11" s="432" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="Z11" s="431" t="s">
         <v>397</v>
@@ -8809,7 +8790,7 @@
       </c>
       <c r="AC11" s="443"/>
       <c r="AD11" s="442" t="s">
-        <v>1116</v>
+        <v>1108</v>
       </c>
       <c r="AE11" s="446"/>
       <c r="AF11" s="444" t="s">
@@ -8890,19 +8871,17 @@
       <c r="C12" s="97" t="s">
         <v>412</v>
       </c>
-      <c r="D12" s="632" t="s">
-        <v>1131</v>
-      </c>
+      <c r="D12" s="632"/>
       <c r="E12" s="90" t="s">
         <v>391</v>
       </c>
       <c r="F12" s="410" t="s">
-        <v>1048</v>
+        <v>753</v>
       </c>
       <c r="G12" s="461"/>
       <c r="H12" s="472"/>
       <c r="I12" s="409" t="s">
-        <v>1052</v>
+        <v>1090</v>
       </c>
       <c r="J12" s="43" t="s">
         <v>393</v>
@@ -8914,7 +8893,7 @@
         <v>394</v>
       </c>
       <c r="M12" s="409" t="s">
-        <v>1063</v>
+        <v>1094</v>
       </c>
       <c r="N12" s="446" t="s">
         <v>562</v>
@@ -8926,7 +8905,7 @@
         <v>409</v>
       </c>
       <c r="Q12" s="409" t="s">
-        <v>1076</v>
+        <v>1098</v>
       </c>
       <c r="R12" s="419" t="s">
         <v>586</v>
@@ -8938,7 +8917,7 @@
         <v>562</v>
       </c>
       <c r="U12" s="420" t="s">
-        <v>1090</v>
+        <v>1102</v>
       </c>
       <c r="V12" s="90" t="s">
         <v>850</v>
@@ -8950,7 +8929,7 @@
         <v>396</v>
       </c>
       <c r="Y12" s="432" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="Z12" s="430" t="s">
         <v>397</v>
@@ -8965,7 +8944,7 @@
         <v>570</v>
       </c>
       <c r="AD12" s="442" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
       <c r="AE12" s="446"/>
       <c r="AF12" s="101" t="s">
@@ -9049,21 +9028,19 @@
       <c r="C13" s="97" t="s">
         <v>413</v>
       </c>
-      <c r="D13" s="632" t="s">
-        <v>1132</v>
-      </c>
+      <c r="D13" s="632"/>
       <c r="E13" s="90" t="s">
         <v>391</v>
       </c>
       <c r="F13" s="410" t="s">
-        <v>1048</v>
+        <v>753</v>
       </c>
       <c r="G13" s="461" t="s">
         <v>392</v>
       </c>
       <c r="H13" s="472"/>
       <c r="I13" s="409" t="s">
-        <v>1053</v>
+        <v>1091</v>
       </c>
       <c r="J13" s="43" t="s">
         <v>393</v>
@@ -9075,7 +9052,7 @@
         <v>394</v>
       </c>
       <c r="M13" s="409" t="s">
-        <v>1064</v>
+        <v>1095</v>
       </c>
       <c r="N13" s="446" t="s">
         <v>562</v>
@@ -9087,7 +9064,7 @@
         <v>409</v>
       </c>
       <c r="Q13" s="409" t="s">
-        <v>1077</v>
+        <v>1099</v>
       </c>
       <c r="R13" s="419" t="s">
         <v>587</v>
@@ -9099,7 +9076,7 @@
         <v>562</v>
       </c>
       <c r="U13" s="420" t="s">
-        <v>1091</v>
+        <v>1103</v>
       </c>
       <c r="V13" s="90" t="s">
         <v>851</v>
@@ -9111,7 +9088,7 @@
         <v>396</v>
       </c>
       <c r="Y13" s="432" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="Z13" s="430" t="s">
         <v>397</v>
@@ -9126,7 +9103,7 @@
         <v>591</v>
       </c>
       <c r="AD13" s="442" t="s">
-        <v>1118</v>
+        <v>1111</v>
       </c>
       <c r="AE13" s="358"/>
       <c r="AF13" s="101" t="s">
@@ -9224,7 +9201,7 @@
       <c r="G14" s="44"/>
       <c r="H14" s="45"/>
       <c r="I14" s="381" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="J14" s="43" t="s">
         <v>393</v>
@@ -9236,7 +9213,7 @@
         <v>394</v>
       </c>
       <c r="M14" s="409" t="s">
-        <v>1065</v>
+        <v>1054</v>
       </c>
       <c r="N14" s="106" t="s">
         <v>562</v>
@@ -9248,7 +9225,7 @@
         <v>409</v>
       </c>
       <c r="Q14" s="409" t="s">
-        <v>1078</v>
+        <v>1061</v>
       </c>
       <c r="R14" s="92" t="s">
         <v>603</v>
@@ -9260,7 +9237,7 @@
         <v>562</v>
       </c>
       <c r="U14" s="420" t="s">
-        <v>1092</v>
+        <v>1069</v>
       </c>
       <c r="V14" s="90" t="s">
         <v>852</v>
@@ -9272,7 +9249,7 @@
         <v>905</v>
       </c>
       <c r="Y14" s="432" t="s">
-        <v>1105</v>
+        <v>1076</v>
       </c>
       <c r="Z14" s="93" t="s">
         <v>397</v>
@@ -9287,7 +9264,7 @@
         <v>593</v>
       </c>
       <c r="AD14" s="380" t="s">
-        <v>1119</v>
+        <v>1112</v>
       </c>
       <c r="AE14" s="106"/>
       <c r="AF14" s="101" t="s">
@@ -9384,7 +9361,7 @@
       <c r="G15" s="461"/>
       <c r="H15" s="472"/>
       <c r="I15" s="381" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
       <c r="J15" s="43" t="s">
         <v>393</v>
@@ -9396,7 +9373,7 @@
         <v>394</v>
       </c>
       <c r="M15" s="409" t="s">
-        <v>1066</v>
+        <v>1055</v>
       </c>
       <c r="N15" s="446" t="s">
         <v>562</v>
@@ -9408,7 +9385,7 @@
         <v>409</v>
       </c>
       <c r="Q15" s="409" t="s">
-        <v>1079</v>
+        <v>1062</v>
       </c>
       <c r="R15" s="419" t="s">
         <v>605</v>
@@ -9420,7 +9397,7 @@
         <v>562</v>
       </c>
       <c r="U15" s="420" t="s">
-        <v>1093</v>
+        <v>1070</v>
       </c>
       <c r="V15" s="90" t="s">
         <v>853</v>
@@ -9432,7 +9409,7 @@
         <v>396</v>
       </c>
       <c r="Y15" s="432" t="s">
-        <v>1106</v>
+        <v>1077</v>
       </c>
       <c r="Z15" s="430" t="s">
         <v>397</v>
@@ -9447,7 +9424,7 @@
         <v>607</v>
       </c>
       <c r="AD15" s="442" t="s">
-        <v>1120</v>
+        <v>1084</v>
       </c>
       <c r="AE15" s="446"/>
       <c r="AF15" s="101" t="s">
@@ -9549,7 +9526,7 @@
         <v>394</v>
       </c>
       <c r="M16" s="409" t="s">
-        <v>1067</v>
+        <v>1056</v>
       </c>
       <c r="N16" s="106" t="s">
         <v>562</v>
@@ -9561,7 +9538,7 @@
         <v>409</v>
       </c>
       <c r="Q16" s="409" t="s">
-        <v>1080</v>
+        <v>1063</v>
       </c>
       <c r="R16" s="419" t="s">
         <v>892</v>
@@ -9573,7 +9550,7 @@
         <v>562</v>
       </c>
       <c r="U16" s="420" t="s">
-        <v>1094</v>
+        <v>1071</v>
       </c>
       <c r="V16" s="90" t="s">
         <v>893</v>
@@ -9583,7 +9560,7 @@
         <v>905</v>
       </c>
       <c r="Y16" s="432" t="s">
-        <v>1107</v>
+        <v>1078</v>
       </c>
       <c r="Z16" s="93" t="s">
         <v>397</v>
@@ -9596,7 +9573,7 @@
       </c>
       <c r="AC16" s="100"/>
       <c r="AD16" s="380" t="s">
-        <v>1121</v>
+        <v>1108</v>
       </c>
       <c r="AE16" s="106"/>
       <c r="AF16" s="101" t="s">
@@ -9690,7 +9667,7 @@
       <c r="G17" s="44"/>
       <c r="H17" s="45"/>
       <c r="I17" s="381" t="s">
-        <v>1056</v>
+        <v>1051</v>
       </c>
       <c r="J17" s="43" t="s">
         <v>393</v>
@@ -9702,7 +9679,7 @@
         <v>394</v>
       </c>
       <c r="M17" s="409" t="s">
-        <v>1068</v>
+        <v>1057</v>
       </c>
       <c r="N17" s="106" t="s">
         <v>562</v>
@@ -9714,7 +9691,7 @@
         <v>409</v>
       </c>
       <c r="Q17" s="409" t="s">
-        <v>1081</v>
+        <v>1064</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>902</v>
@@ -9726,7 +9703,7 @@
         <v>562</v>
       </c>
       <c r="U17" s="420" t="s">
-        <v>1095</v>
+        <v>1072</v>
       </c>
       <c r="V17" s="90" t="s">
         <v>893</v>
@@ -9736,7 +9713,7 @@
         <v>904</v>
       </c>
       <c r="Y17" s="432" t="s">
-        <v>1108</v>
+        <v>1079</v>
       </c>
       <c r="Z17" s="93" t="s">
         <v>397</v>
@@ -9751,7 +9728,7 @@
         <v>570</v>
       </c>
       <c r="AD17" s="380" t="s">
-        <v>1122</v>
+        <v>1084</v>
       </c>
       <c r="AE17" s="106"/>
       <c r="AF17" s="101" t="s">
@@ -9843,7 +9820,7 @@
       <c r="G18" s="44"/>
       <c r="H18" s="45"/>
       <c r="I18" s="381" t="s">
-        <v>1057</v>
+        <v>1052</v>
       </c>
       <c r="J18" s="43" t="s">
         <v>910</v>
@@ -9855,7 +9832,7 @@
         <v>918</v>
       </c>
       <c r="M18" s="409" t="s">
-        <v>1070</v>
+        <v>1059</v>
       </c>
       <c r="N18" s="106" t="s">
         <v>562</v>
@@ -9867,7 +9844,7 @@
         <v>409</v>
       </c>
       <c r="Q18" s="409" t="s">
-        <v>1082</v>
+        <v>1065</v>
       </c>
       <c r="R18" s="92" t="s">
         <v>603</v>
@@ -9879,7 +9856,7 @@
         <v>562</v>
       </c>
       <c r="U18" s="420" t="s">
-        <v>1096</v>
+        <v>1073</v>
       </c>
       <c r="V18" s="90" t="s">
         <v>893</v>
@@ -9891,7 +9868,7 @@
         <v>905</v>
       </c>
       <c r="Y18" s="432" t="s">
-        <v>1109</v>
+        <v>1080</v>
       </c>
       <c r="Z18" s="93" t="s">
         <v>397</v>
@@ -9906,7 +9883,7 @@
         <v>570</v>
       </c>
       <c r="AD18" s="380" t="s">
-        <v>1123</v>
+        <v>1085</v>
       </c>
       <c r="AE18" s="106"/>
       <c r="AF18" s="101" t="s">
@@ -9998,7 +9975,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="45"/>
       <c r="I19" s="381" t="s">
-        <v>1058</v>
+        <v>1053</v>
       </c>
       <c r="J19" s="43" t="s">
         <v>393</v>
@@ -10010,7 +9987,7 @@
         <v>918</v>
       </c>
       <c r="M19" s="409" t="s">
-        <v>1069</v>
+        <v>1058</v>
       </c>
       <c r="N19" s="106" t="s">
         <v>562</v>
@@ -10022,7 +9999,7 @@
         <v>409</v>
       </c>
       <c r="Q19" s="409" t="s">
-        <v>1083</v>
+        <v>1066</v>
       </c>
       <c r="R19" s="92" t="s">
         <v>603</v>
@@ -10046,7 +10023,7 @@
         <v>905</v>
       </c>
       <c r="Y19" s="432" t="s">
-        <v>1110</v>
+        <v>1081</v>
       </c>
       <c r="Z19" s="93" t="s">
         <v>397</v>
@@ -10061,7 +10038,7 @@
         <v>570</v>
       </c>
       <c r="AD19" s="380" t="s">
-        <v>1124</v>
+        <v>1086</v>
       </c>
       <c r="AE19" s="106"/>
       <c r="AF19" s="101" t="s">
@@ -10165,7 +10142,7 @@
         <v>918</v>
       </c>
       <c r="M20" s="409" t="s">
-        <v>1071</v>
+        <v>1060</v>
       </c>
       <c r="N20" s="106" t="s">
         <v>562</v>
@@ -10177,7 +10154,7 @@
         <v>409</v>
       </c>
       <c r="Q20" s="409" t="s">
-        <v>1084</v>
+        <v>1067</v>
       </c>
       <c r="R20" s="92" t="s">
         <v>931</v>
@@ -10189,7 +10166,7 @@
         <v>562</v>
       </c>
       <c r="U20" s="420" t="s">
-        <v>1097</v>
+        <v>1074</v>
       </c>
       <c r="V20" s="90" t="s">
         <v>926</v>
@@ -10201,7 +10178,7 @@
         <v>396</v>
       </c>
       <c r="Y20" s="432" t="s">
-        <v>1111</v>
+        <v>1082</v>
       </c>
       <c r="Z20" s="93" t="s">
         <v>397</v>
@@ -10216,7 +10193,7 @@
         <v>932</v>
       </c>
       <c r="AD20" s="380" t="s">
-        <v>1125</v>
+        <v>1087</v>
       </c>
       <c r="AE20" s="106"/>
       <c r="AF20" s="101" t="s">
@@ -10336,7 +10313,7 @@
         <v>409</v>
       </c>
       <c r="Q21" s="564" t="s">
-        <v>1085</v>
+        <v>1068</v>
       </c>
       <c r="R21" s="92" t="s">
         <v>934</v>
@@ -10348,7 +10325,7 @@
         <v>562</v>
       </c>
       <c r="U21" s="566" t="s">
-        <v>1098</v>
+        <v>1075</v>
       </c>
       <c r="V21" s="559" t="s">
         <v>926</v>
@@ -10360,7 +10337,7 @@
         <v>396</v>
       </c>
       <c r="Y21" s="567" t="s">
-        <v>1112</v>
+        <v>1083</v>
       </c>
       <c r="Z21" s="568" t="s">
         <v>397</v>
@@ -10375,7 +10352,7 @@
         <v>935</v>
       </c>
       <c r="AD21" s="572" t="s">
-        <v>1126</v>
+        <v>1088</v>
       </c>
       <c r="AE21" s="565"/>
       <c r="AF21" s="573" t="s">

</xml_diff>

<commit_message>
[MaintainBooking] : Screenshot Script Added
</commit_message>
<xml_diff>
--- a/InputData/BookingData.xlsx
+++ b/InputData/BookingData.xlsx
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="1126">
   <si>
     <t>ID</t>
   </si>
@@ -3720,253 +3720,247 @@
     <t>112-329-7806</t>
   </si>
   <si>
-    <t>26-Jun-2023</t>
-  </si>
-  <si>
     <t>49009</t>
   </si>
   <si>
+    <t>21-Jun-2023</t>
+  </si>
+  <si>
+    <t>125-368-2568</t>
+  </si>
+  <si>
+    <t>232-369-3654</t>
+  </si>
+  <si>
+    <t>232-370-607</t>
+  </si>
+  <si>
+    <t>232-371-548</t>
+  </si>
+  <si>
+    <t>232-372-956</t>
+  </si>
+  <si>
+    <t>4523850</t>
+  </si>
+  <si>
+    <t>451051</t>
+  </si>
+  <si>
+    <t>450252</t>
+  </si>
+  <si>
+    <t>456753</t>
+  </si>
+  <si>
+    <t>451255</t>
+  </si>
+  <si>
+    <t>453954</t>
+  </si>
+  <si>
+    <t>451856</t>
+  </si>
+  <si>
+    <t>AAS1249</t>
+  </si>
+  <si>
+    <t>BB11250</t>
+  </si>
+  <si>
+    <t>BB11051</t>
+  </si>
+  <si>
+    <t>BB11052</t>
+  </si>
+  <si>
+    <t>BB11853</t>
+  </si>
+  <si>
+    <t>BB11854</t>
+  </si>
+  <si>
+    <t>BB11855</t>
+  </si>
+  <si>
+    <t>BB30056</t>
+  </si>
+  <si>
+    <t>ICICI00066791</t>
+  </si>
+  <si>
+    <t>ICICI00073592</t>
+  </si>
+  <si>
+    <t>ICICI0006793</t>
+  </si>
+  <si>
+    <t>ICICI00003294</t>
+  </si>
+  <si>
+    <t>ICICI0003995</t>
+  </si>
+  <si>
+    <t>ICICI0000197</t>
+  </si>
+  <si>
+    <t>ICICI0008898</t>
+  </si>
+  <si>
+    <t>353307</t>
+  </si>
+  <si>
+    <t>340308</t>
+  </si>
+  <si>
+    <t>345309</t>
+  </si>
+  <si>
+    <t>345310</t>
+  </si>
+  <si>
+    <t>3448011</t>
+  </si>
+  <si>
+    <t>3424812</t>
+  </si>
+  <si>
+    <t>343113</t>
+  </si>
+  <si>
+    <t>3463514</t>
+  </si>
+  <si>
+    <t>PF/PR/672/2023</t>
+  </si>
+  <si>
+    <t>PF/PP/673/2023</t>
+  </si>
+  <si>
+    <t>PF/PP/674/2023</t>
+  </si>
+  <si>
+    <t>PF/PP/675/2023</t>
+  </si>
+  <si>
+    <t>PF/AP/676/2023</t>
+  </si>
+  <si>
+    <t>458-373-3654</t>
+  </si>
+  <si>
+    <t>258-374-3657</t>
+  </si>
+  <si>
+    <t>457554</t>
+  </si>
+  <si>
+    <t>426555</t>
+  </si>
+  <si>
+    <t>1HG854</t>
+  </si>
+  <si>
+    <t>1267955</t>
+  </si>
+  <si>
+    <t>ICICI00063594</t>
+  </si>
+  <si>
+    <t>ICICI00072395</t>
+  </si>
+  <si>
+    <t>323510</t>
+  </si>
+  <si>
+    <t>396711</t>
+  </si>
+  <si>
+    <t>PF/PR/673/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/674/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/675/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/676/2023</t>
+  </si>
+  <si>
     <t>28-Jun-2023</t>
   </si>
   <si>
-    <t>21-Jun-2023</t>
-  </si>
-  <si>
-    <t>125-368-2568</t>
-  </si>
-  <si>
-    <t>232-369-3654</t>
-  </si>
-  <si>
-    <t>232-370-607</t>
-  </si>
-  <si>
-    <t>232-371-548</t>
-  </si>
-  <si>
-    <t>232-372-956</t>
-  </si>
-  <si>
-    <t>4523850</t>
-  </si>
-  <si>
-    <t>451051</t>
-  </si>
-  <si>
-    <t>450252</t>
-  </si>
-  <si>
-    <t>456753</t>
-  </si>
-  <si>
-    <t>451255</t>
-  </si>
-  <si>
-    <t>453954</t>
-  </si>
-  <si>
-    <t>451856</t>
-  </si>
-  <si>
-    <t>AAS1249</t>
-  </si>
-  <si>
-    <t>BB11250</t>
-  </si>
-  <si>
-    <t>BB11051</t>
-  </si>
-  <si>
-    <t>BB11052</t>
-  </si>
-  <si>
-    <t>BB11853</t>
-  </si>
-  <si>
-    <t>BB11854</t>
-  </si>
-  <si>
-    <t>BB11855</t>
-  </si>
-  <si>
-    <t>BB30056</t>
-  </si>
-  <si>
-    <t>ICICI00066791</t>
-  </si>
-  <si>
-    <t>ICICI00073592</t>
-  </si>
-  <si>
-    <t>ICICI0006793</t>
-  </si>
-  <si>
-    <t>ICICI00003294</t>
-  </si>
-  <si>
-    <t>ICICI0003995</t>
-  </si>
-  <si>
-    <t>ICICI0000197</t>
-  </si>
-  <si>
-    <t>ICICI0008898</t>
-  </si>
-  <si>
-    <t>353307</t>
-  </si>
-  <si>
-    <t>340308</t>
-  </si>
-  <si>
-    <t>345309</t>
-  </si>
-  <si>
-    <t>345310</t>
-  </si>
-  <si>
-    <t>3448011</t>
-  </si>
-  <si>
-    <t>3424812</t>
-  </si>
-  <si>
-    <t>343113</t>
-  </si>
-  <si>
-    <t>3463514</t>
-  </si>
-  <si>
-    <t>PF/PR/672/2023</t>
-  </si>
-  <si>
-    <t>PF/PP/673/2023</t>
-  </si>
-  <si>
-    <t>PF/PP/674/2023</t>
-  </si>
-  <si>
-    <t>PF/PP/675/2023</t>
-  </si>
-  <si>
-    <t>PF/AP/676/2023</t>
-  </si>
-  <si>
-    <t>232-372-2587</t>
-  </si>
-  <si>
-    <t>458-373-3654</t>
-  </si>
-  <si>
-    <t>258-374-3657</t>
-  </si>
-  <si>
-    <t>42652</t>
-  </si>
-  <si>
-    <t>477153</t>
-  </si>
-  <si>
-    <t>457554</t>
-  </si>
-  <si>
-    <t>426555</t>
-  </si>
-  <si>
-    <t>535352</t>
-  </si>
-  <si>
-    <t>166253</t>
-  </si>
-  <si>
-    <t>1HG854</t>
-  </si>
-  <si>
-    <t>1267955</t>
-  </si>
-  <si>
-    <t>ICICI0000892</t>
-  </si>
-  <si>
-    <t>ICICI0000693</t>
-  </si>
-  <si>
-    <t>ICICI00063594</t>
-  </si>
-  <si>
-    <t>ICICI00072395</t>
-  </si>
-  <si>
-    <t>345808</t>
-  </si>
-  <si>
-    <t>324609</t>
-  </si>
-  <si>
-    <t>323510</t>
-  </si>
-  <si>
-    <t>396711</t>
-  </si>
-  <si>
-    <t>PF/PR/673/2023</t>
-  </si>
-  <si>
-    <t>PF/SA/672/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/674/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/675/2023</t>
-  </si>
-  <si>
-    <t>PF/PR/676/2023</t>
-  </si>
-  <si>
-    <t>890-374-6027</t>
-  </si>
-  <si>
-    <t>232-375-9631</t>
-  </si>
-  <si>
-    <t>29-Jun-2023</t>
-  </si>
-  <si>
-    <t>25054</t>
-  </si>
-  <si>
-    <t>43055</t>
-  </si>
-  <si>
-    <t>820054</t>
-  </si>
-  <si>
-    <t>180055</t>
-  </si>
-  <si>
-    <t>ICICI0000894</t>
-  </si>
-  <si>
-    <t>ICICI0000895</t>
-  </si>
-  <si>
-    <t>833808</t>
-  </si>
-  <si>
-    <t>353409</t>
-  </si>
-  <si>
-    <t>PF/RD/674/2023</t>
-  </si>
-  <si>
-    <t>PF/HE/675/2023</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFE/00179/23-24</t>
-  </si>
-  <si>
-    <t>MUM/BKG/AEC/00012/2122-51</t>
+    <t>232-394-2587</t>
+  </si>
+  <si>
+    <t>42677</t>
+  </si>
+  <si>
+    <t>47778</t>
+  </si>
+  <si>
+    <t>535377</t>
+  </si>
+  <si>
+    <t>166278</t>
+  </si>
+  <si>
+    <t>ICICI0000117</t>
+  </si>
+  <si>
+    <t>ICICI0000118</t>
+  </si>
+  <si>
+    <t>345831</t>
+  </si>
+  <si>
+    <t>324632</t>
+  </si>
+  <si>
+    <t>PF/SA/697/2023</t>
+  </si>
+  <si>
+    <t>PF/PR/698/2023</t>
+  </si>
+  <si>
+    <t>03-Jul-2023</t>
+  </si>
+  <si>
+    <t>232-396-9631</t>
+  </si>
+  <si>
+    <t>15-Jul-2023</t>
+  </si>
+  <si>
+    <t>43079</t>
+  </si>
+  <si>
+    <t>180080</t>
+  </si>
+  <si>
+    <t>ICICI0000120</t>
+  </si>
+  <si>
+    <t>353434</t>
+  </si>
+  <si>
+    <t>PF/HE/700/2023</t>
+  </si>
+  <si>
+    <t>890-397-6027</t>
+  </si>
+  <si>
+    <t>820082</t>
+  </si>
+  <si>
+    <t>PF/RD/701/2023</t>
+  </si>
+  <si>
+    <t>25081</t>
+  </si>
+  <si>
+    <t>833836</t>
   </si>
 </sst>
 </file>
@@ -4165,6 +4159,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -7450,7 +7445,7 @@
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8:D9"/>
+      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8231,19 +8226,17 @@
       <c r="C8" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="717" t="s">
-        <v>1126</v>
-      </c>
+      <c r="D8" s="717"/>
       <c r="E8" s="215" t="s">
         <v>391</v>
       </c>
       <c r="F8" s="394" t="s">
-        <v>1045</v>
+        <v>1113</v>
       </c>
       <c r="G8" s="216"/>
       <c r="H8" s="399"/>
       <c r="I8" s="451" t="s">
-        <v>1113</v>
+        <v>1121</v>
       </c>
       <c r="J8" s="219" t="s">
         <v>393</v>
@@ -8255,7 +8248,7 @@
         <v>394</v>
       </c>
       <c r="M8" s="451" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="N8" s="220" t="s">
         <v>562</v>
@@ -8267,7 +8260,7 @@
         <v>409</v>
       </c>
       <c r="Q8" s="451" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
       <c r="R8" s="465" t="s">
         <v>727</v>
@@ -8279,7 +8272,7 @@
         <v>562</v>
       </c>
       <c r="U8" s="426" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="V8" s="425" t="s">
         <v>854</v>
@@ -8291,7 +8284,7 @@
         <v>396</v>
       </c>
       <c r="Y8" s="434" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="Z8" s="435" t="s">
         <v>397</v>
@@ -8306,7 +8299,7 @@
         <v>561</v>
       </c>
       <c r="AD8" s="450" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="AE8" s="452"/>
       <c r="AF8" s="451" t="s">
@@ -8399,14 +8392,12 @@
       <c r="C9" s="288" t="s">
         <v>410</v>
       </c>
-      <c r="D9" s="714" t="s">
-        <v>1127</v>
-      </c>
+      <c r="D9" s="714"/>
       <c r="E9" s="122" t="s">
         <v>391</v>
       </c>
       <c r="F9" s="396" t="s">
-        <v>1045</v>
+        <v>1113</v>
       </c>
       <c r="G9" s="289"/>
       <c r="H9" s="401" t="s">
@@ -8419,13 +8410,13 @@
         <v>393</v>
       </c>
       <c r="K9" s="407" t="s">
-        <v>1047</v>
+        <v>752</v>
       </c>
       <c r="L9" s="408" t="s">
         <v>394</v>
       </c>
       <c r="M9" s="411" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="N9" s="291" t="s">
         <v>562</v>
@@ -8437,7 +8428,7 @@
         <v>409</v>
       </c>
       <c r="Q9" s="411" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="R9" s="421" t="s">
         <v>395</v>
@@ -8449,7 +8440,7 @@
         <v>562</v>
       </c>
       <c r="U9" s="429" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="V9" s="423" t="s">
         <v>847</v>
@@ -8459,7 +8450,7 @@
         <v>396</v>
       </c>
       <c r="Y9" s="439" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="Z9" s="440" t="s">
         <v>397</v>
@@ -8472,7 +8463,7 @@
       </c>
       <c r="AC9" s="459"/>
       <c r="AD9" s="448" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="AE9" s="458"/>
       <c r="AF9" s="460" t="s">
@@ -8570,12 +8561,12 @@
         <v>391</v>
       </c>
       <c r="F10" s="395" t="s">
-        <v>753</v>
+        <v>657</v>
       </c>
       <c r="G10" s="277"/>
       <c r="H10" s="400"/>
       <c r="I10" s="397" t="s">
-        <v>1089</v>
+        <v>1102</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>393</v>
@@ -8587,7 +8578,7 @@
         <v>394</v>
       </c>
       <c r="M10" s="412" t="s">
-        <v>1092</v>
+        <v>1103</v>
       </c>
       <c r="N10" s="279" t="s">
         <v>562</v>
@@ -8599,7 +8590,7 @@
         <v>409</v>
       </c>
       <c r="Q10" s="412" t="s">
-        <v>1096</v>
+        <v>1105</v>
       </c>
       <c r="R10" s="422" t="s">
         <v>395</v>
@@ -8611,7 +8602,7 @@
         <v>562</v>
       </c>
       <c r="U10" s="428" t="s">
-        <v>1100</v>
+        <v>1107</v>
       </c>
       <c r="V10" s="424" t="s">
         <v>848</v>
@@ -8623,7 +8614,7 @@
         <v>396</v>
       </c>
       <c r="Y10" s="436" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="Z10" s="437" t="s">
         <v>397</v>
@@ -8638,7 +8629,7 @@
         <v>1025</v>
       </c>
       <c r="AD10" s="449" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="AE10" s="454"/>
       <c r="AF10" s="456" t="s">
@@ -8728,7 +8719,7 @@
         <v>391</v>
       </c>
       <c r="F11" s="410" t="s">
-        <v>753</v>
+        <v>657</v>
       </c>
       <c r="G11" s="461"/>
       <c r="H11" s="472" t="s">
@@ -8743,7 +8734,7 @@
         <v>394</v>
       </c>
       <c r="M11" s="409" t="s">
-        <v>1093</v>
+        <v>1104</v>
       </c>
       <c r="N11" s="446" t="s">
         <v>562</v>
@@ -8755,7 +8746,7 @@
         <v>409</v>
       </c>
       <c r="Q11" s="409" t="s">
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="R11" s="419" t="s">
         <v>395</v>
@@ -8767,7 +8758,7 @@
         <v>562</v>
       </c>
       <c r="U11" s="420" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="V11" s="442" t="s">
         <v>849</v>
@@ -8777,7 +8768,7 @@
         <v>396</v>
       </c>
       <c r="Y11" s="432" t="s">
-        <v>1105</v>
+        <v>1110</v>
       </c>
       <c r="Z11" s="431" t="s">
         <v>397</v>
@@ -8790,7 +8781,7 @@
       </c>
       <c r="AC11" s="443"/>
       <c r="AD11" s="442" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="AE11" s="446"/>
       <c r="AF11" s="444" t="s">
@@ -8876,12 +8867,12 @@
         <v>391</v>
       </c>
       <c r="F12" s="410" t="s">
-        <v>753</v>
+        <v>1101</v>
       </c>
       <c r="G12" s="461"/>
       <c r="H12" s="472"/>
       <c r="I12" s="409" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="J12" s="43" t="s">
         <v>393</v>
@@ -8893,7 +8884,7 @@
         <v>394</v>
       </c>
       <c r="M12" s="409" t="s">
-        <v>1094</v>
+        <v>1089</v>
       </c>
       <c r="N12" s="446" t="s">
         <v>562</v>
@@ -8905,7 +8896,7 @@
         <v>409</v>
       </c>
       <c r="Q12" s="409" t="s">
-        <v>1098</v>
+        <v>1091</v>
       </c>
       <c r="R12" s="419" t="s">
         <v>586</v>
@@ -8917,7 +8908,7 @@
         <v>562</v>
       </c>
       <c r="U12" s="420" t="s">
-        <v>1102</v>
+        <v>1093</v>
       </c>
       <c r="V12" s="90" t="s">
         <v>850</v>
@@ -8929,7 +8920,7 @@
         <v>396</v>
       </c>
       <c r="Y12" s="432" t="s">
-        <v>1106</v>
+        <v>1095</v>
       </c>
       <c r="Z12" s="430" t="s">
         <v>397</v>
@@ -8944,7 +8935,7 @@
         <v>570</v>
       </c>
       <c r="AD12" s="442" t="s">
-        <v>1110</v>
+        <v>1098</v>
       </c>
       <c r="AE12" s="446"/>
       <c r="AF12" s="101" t="s">
@@ -9040,7 +9031,7 @@
       </c>
       <c r="H13" s="472"/>
       <c r="I13" s="409" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="J13" s="43" t="s">
         <v>393</v>
@@ -9052,7 +9043,7 @@
         <v>394</v>
       </c>
       <c r="M13" s="409" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
       <c r="N13" s="446" t="s">
         <v>562</v>
@@ -9064,7 +9055,7 @@
         <v>409</v>
       </c>
       <c r="Q13" s="409" t="s">
-        <v>1099</v>
+        <v>1092</v>
       </c>
       <c r="R13" s="419" t="s">
         <v>587</v>
@@ -9076,7 +9067,7 @@
         <v>562</v>
       </c>
       <c r="U13" s="420" t="s">
-        <v>1103</v>
+        <v>1094</v>
       </c>
       <c r="V13" s="90" t="s">
         <v>851</v>
@@ -9088,7 +9079,7 @@
         <v>396</v>
       </c>
       <c r="Y13" s="432" t="s">
-        <v>1107</v>
+        <v>1096</v>
       </c>
       <c r="Z13" s="430" t="s">
         <v>397</v>
@@ -9103,7 +9094,7 @@
         <v>591</v>
       </c>
       <c r="AD13" s="442" t="s">
-        <v>1111</v>
+        <v>1099</v>
       </c>
       <c r="AE13" s="358"/>
       <c r="AF13" s="101" t="s">
@@ -9196,12 +9187,12 @@
         <v>391</v>
       </c>
       <c r="F14" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G14" s="44"/>
       <c r="H14" s="45"/>
       <c r="I14" s="381" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="J14" s="43" t="s">
         <v>393</v>
@@ -9213,7 +9204,7 @@
         <v>394</v>
       </c>
       <c r="M14" s="409" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="N14" s="106" t="s">
         <v>562</v>
@@ -9225,7 +9216,7 @@
         <v>409</v>
       </c>
       <c r="Q14" s="409" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="R14" s="92" t="s">
         <v>603</v>
@@ -9237,7 +9228,7 @@
         <v>562</v>
       </c>
       <c r="U14" s="420" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="V14" s="90" t="s">
         <v>852</v>
@@ -9249,7 +9240,7 @@
         <v>905</v>
       </c>
       <c r="Y14" s="432" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="Z14" s="93" t="s">
         <v>397</v>
@@ -9264,7 +9255,7 @@
         <v>593</v>
       </c>
       <c r="AD14" s="380" t="s">
-        <v>1112</v>
+        <v>1100</v>
       </c>
       <c r="AE14" s="106"/>
       <c r="AF14" s="101" t="s">
@@ -9356,12 +9347,12 @@
         <v>391</v>
       </c>
       <c r="F15" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G15" s="461"/>
       <c r="H15" s="472"/>
       <c r="I15" s="381" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="J15" s="43" t="s">
         <v>393</v>
@@ -9373,7 +9364,7 @@
         <v>394</v>
       </c>
       <c r="M15" s="409" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="N15" s="446" t="s">
         <v>562</v>
@@ -9385,7 +9376,7 @@
         <v>409</v>
       </c>
       <c r="Q15" s="409" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="R15" s="419" t="s">
         <v>605</v>
@@ -9397,7 +9388,7 @@
         <v>562</v>
       </c>
       <c r="U15" s="420" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="V15" s="90" t="s">
         <v>853</v>
@@ -9409,7 +9400,7 @@
         <v>396</v>
       </c>
       <c r="Y15" s="432" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="Z15" s="430" t="s">
         <v>397</v>
@@ -9424,7 +9415,7 @@
         <v>607</v>
       </c>
       <c r="AD15" s="442" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="AE15" s="446"/>
       <c r="AF15" s="101" t="s">
@@ -9513,7 +9504,7 @@
         <v>911</v>
       </c>
       <c r="F16" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G16" s="44"/>
       <c r="H16" s="45"/>
@@ -9526,7 +9517,7 @@
         <v>394</v>
       </c>
       <c r="M16" s="409" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="N16" s="106" t="s">
         <v>562</v>
@@ -9538,7 +9529,7 @@
         <v>409</v>
       </c>
       <c r="Q16" s="409" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="R16" s="419" t="s">
         <v>892</v>
@@ -9550,7 +9541,7 @@
         <v>562</v>
       </c>
       <c r="U16" s="420" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="V16" s="90" t="s">
         <v>893</v>
@@ -9560,7 +9551,7 @@
         <v>905</v>
       </c>
       <c r="Y16" s="432" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="Z16" s="93" t="s">
         <v>397</v>
@@ -9573,7 +9564,7 @@
       </c>
       <c r="AC16" s="100"/>
       <c r="AD16" s="380" t="s">
-        <v>1108</v>
+        <v>1097</v>
       </c>
       <c r="AE16" s="106"/>
       <c r="AF16" s="101" t="s">
@@ -9662,12 +9653,12 @@
         <v>391</v>
       </c>
       <c r="F17" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G17" s="44"/>
       <c r="H17" s="45"/>
       <c r="I17" s="381" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="J17" s="43" t="s">
         <v>393</v>
@@ -9679,7 +9670,7 @@
         <v>394</v>
       </c>
       <c r="M17" s="409" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="N17" s="106" t="s">
         <v>562</v>
@@ -9691,7 +9682,7 @@
         <v>409</v>
       </c>
       <c r="Q17" s="409" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>902</v>
@@ -9703,7 +9694,7 @@
         <v>562</v>
       </c>
       <c r="U17" s="420" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="V17" s="90" t="s">
         <v>893</v>
@@ -9713,7 +9704,7 @@
         <v>904</v>
       </c>
       <c r="Y17" s="432" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="Z17" s="93" t="s">
         <v>397</v>
@@ -9728,7 +9719,7 @@
         <v>570</v>
       </c>
       <c r="AD17" s="380" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="AE17" s="106"/>
       <c r="AF17" s="101" t="s">
@@ -9815,12 +9806,12 @@
         <v>911</v>
       </c>
       <c r="F18" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G18" s="44"/>
       <c r="H18" s="45"/>
       <c r="I18" s="381" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="J18" s="43" t="s">
         <v>910</v>
@@ -9832,7 +9823,7 @@
         <v>918</v>
       </c>
       <c r="M18" s="409" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="N18" s="106" t="s">
         <v>562</v>
@@ -9844,7 +9835,7 @@
         <v>409</v>
       </c>
       <c r="Q18" s="409" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="R18" s="92" t="s">
         <v>603</v>
@@ -9856,7 +9847,7 @@
         <v>562</v>
       </c>
       <c r="U18" s="420" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="V18" s="90" t="s">
         <v>893</v>
@@ -9868,7 +9859,7 @@
         <v>905</v>
       </c>
       <c r="Y18" s="432" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="Z18" s="93" t="s">
         <v>397</v>
@@ -9883,7 +9874,7 @@
         <v>570</v>
       </c>
       <c r="AD18" s="380" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="AE18" s="106"/>
       <c r="AF18" s="101" t="s">
@@ -9970,12 +9961,12 @@
         <v>911</v>
       </c>
       <c r="F19" s="410" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G19" s="44"/>
       <c r="H19" s="45"/>
       <c r="I19" s="381" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="J19" s="43" t="s">
         <v>393</v>
@@ -9987,7 +9978,7 @@
         <v>918</v>
       </c>
       <c r="M19" s="409" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="N19" s="106" t="s">
         <v>562</v>
@@ -9999,7 +9990,7 @@
         <v>409</v>
       </c>
       <c r="Q19" s="409" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="R19" s="92" t="s">
         <v>603</v>
@@ -10023,7 +10014,7 @@
         <v>905</v>
       </c>
       <c r="Y19" s="432" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="Z19" s="93" t="s">
         <v>397</v>
@@ -10038,7 +10029,7 @@
         <v>570</v>
       </c>
       <c r="AD19" s="380" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="AE19" s="106"/>
       <c r="AF19" s="101" t="s">
@@ -10142,7 +10133,7 @@
         <v>918</v>
       </c>
       <c r="M20" s="409" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="N20" s="106" t="s">
         <v>562</v>
@@ -10154,7 +10145,7 @@
         <v>409</v>
       </c>
       <c r="Q20" s="409" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="R20" s="92" t="s">
         <v>931</v>
@@ -10166,7 +10157,7 @@
         <v>562</v>
       </c>
       <c r="U20" s="420" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="V20" s="90" t="s">
         <v>926</v>
@@ -10178,7 +10169,7 @@
         <v>396</v>
       </c>
       <c r="Y20" s="432" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="Z20" s="93" t="s">
         <v>397</v>
@@ -10193,7 +10184,7 @@
         <v>932</v>
       </c>
       <c r="AD20" s="380" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="AE20" s="106"/>
       <c r="AF20" s="101" t="s">
@@ -10301,7 +10292,7 @@
         <v>918</v>
       </c>
       <c r="M21" s="564" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="N21" s="565" t="s">
         <v>562</v>
@@ -10313,7 +10304,7 @@
         <v>409</v>
       </c>
       <c r="Q21" s="564" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="R21" s="92" t="s">
         <v>934</v>
@@ -10325,7 +10316,7 @@
         <v>562</v>
       </c>
       <c r="U21" s="566" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="V21" s="559" t="s">
         <v>926</v>
@@ -10337,7 +10328,7 @@
         <v>396</v>
       </c>
       <c r="Y21" s="567" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="Z21" s="568" t="s">
         <v>397</v>
@@ -10352,7 +10343,7 @@
         <v>935</v>
       </c>
       <c r="AD21" s="572" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="AE21" s="565"/>
       <c r="AF21" s="573" t="s">
@@ -14519,7 +14510,7 @@
   <dimension ref="A1:GI134"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15239,7 +15230,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="247">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8" s="256" t="s">
         <v>23</v>
@@ -15361,7 +15352,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="486">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" s="487" t="s">
         <v>29</v>
@@ -15381,8 +15372,8 @@
       <c r="H10" s="614" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="487" t="s">
-        <v>395</v>
+      <c r="I10" s="256" t="s">
+        <v>727</v>
       </c>
       <c r="J10" s="488">
         <v>120.23</v>
@@ -15400,8 +15391,8 @@
       <c r="O10" s="623" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="624" t="s">
-        <v>970</v>
+      <c r="P10" s="483" t="s">
+        <v>730</v>
       </c>
       <c r="Q10" s="490">
         <v>140.25</v>

</xml_diff>

<commit_message>
[MaintainBooking] : Upadate Test Data
</commit_message>
<xml_diff>
--- a/InputData/BookingData.xlsx
+++ b/InputData/BookingData.xlsx
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="1124">
   <si>
     <t>ID</t>
   </si>
@@ -3663,18 +3663,12 @@
     <t>AAS789</t>
   </si>
   <si>
-    <t>11-Jul-2023</t>
-  </si>
-  <si>
     <t>AIRLINE CARGO INDIA PVT LTD</t>
   </si>
   <si>
     <t>24-Jun-2023</t>
   </si>
   <si>
-    <t>16-Jul-2023</t>
-  </si>
-  <si>
     <t>23-Jul-2023</t>
   </si>
   <si>
@@ -3924,43 +3918,43 @@
     <t>PF/PR/698/2023</t>
   </si>
   <si>
-    <t>03-Jul-2023</t>
-  </si>
-  <si>
-    <t>232-396-9631</t>
-  </si>
-  <si>
-    <t>15-Jul-2023</t>
-  </si>
-  <si>
-    <t>43079</t>
-  </si>
-  <si>
-    <t>180080</t>
-  </si>
-  <si>
-    <t>ICICI0000120</t>
-  </si>
-  <si>
-    <t>353434</t>
-  </si>
-  <si>
-    <t>PF/HE/700/2023</t>
-  </si>
-  <si>
-    <t>890-397-6027</t>
-  </si>
-  <si>
-    <t>820082</t>
-  </si>
-  <si>
-    <t>PF/RD/701/2023</t>
-  </si>
-  <si>
-    <t>25081</t>
-  </si>
-  <si>
-    <t>833836</t>
+    <t>890-402-6027</t>
+  </si>
+  <si>
+    <t>232-403-9631</t>
+  </si>
+  <si>
+    <t>25086</t>
+  </si>
+  <si>
+    <t>43087</t>
+  </si>
+  <si>
+    <t>820087</t>
+  </si>
+  <si>
+    <t>180088</t>
+  </si>
+  <si>
+    <t>ICICI0000125</t>
+  </si>
+  <si>
+    <t>ICICI0000126</t>
+  </si>
+  <si>
+    <t>833841</t>
+  </si>
+  <si>
+    <t>353442</t>
+  </si>
+  <si>
+    <t>PF/RD/706/2023</t>
+  </si>
+  <si>
+    <t>PF/HE/707/2023</t>
+  </si>
+  <si>
+    <t>30-Jul-2023</t>
   </si>
 </sst>
 </file>
@@ -7445,7 +7439,7 @@
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8231,36 +8225,36 @@
         <v>391</v>
       </c>
       <c r="F8" s="394" t="s">
-        <v>1113</v>
+        <v>769</v>
       </c>
       <c r="G8" s="216"/>
       <c r="H8" s="399"/>
       <c r="I8" s="451" t="s">
-        <v>1121</v>
+        <v>1111</v>
       </c>
       <c r="J8" s="219" t="s">
         <v>393</v>
       </c>
       <c r="K8" s="403" t="s">
-        <v>1115</v>
+        <v>789</v>
       </c>
       <c r="L8" s="404" t="s">
         <v>394</v>
       </c>
       <c r="M8" s="451" t="s">
-        <v>1124</v>
+        <v>1113</v>
       </c>
       <c r="N8" s="220" t="s">
         <v>562</v>
       </c>
       <c r="O8" s="413" t="s">
-        <v>1029</v>
+        <v>1123</v>
       </c>
       <c r="P8" s="414" t="s">
         <v>409</v>
       </c>
       <c r="Q8" s="451" t="s">
-        <v>1122</v>
+        <v>1115</v>
       </c>
       <c r="R8" s="465" t="s">
         <v>727</v>
@@ -8272,7 +8266,7 @@
         <v>562</v>
       </c>
       <c r="U8" s="426" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="V8" s="425" t="s">
         <v>854</v>
@@ -8284,7 +8278,7 @@
         <v>396</v>
       </c>
       <c r="Y8" s="434" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="Z8" s="435" t="s">
         <v>397</v>
@@ -8299,7 +8293,7 @@
         <v>561</v>
       </c>
       <c r="AD8" s="450" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="AE8" s="452"/>
       <c r="AF8" s="451" t="s">
@@ -8397,14 +8391,14 @@
         <v>391</v>
       </c>
       <c r="F9" s="396" t="s">
-        <v>1113</v>
+        <v>769</v>
       </c>
       <c r="G9" s="289"/>
       <c r="H9" s="401" t="s">
         <v>574</v>
       </c>
       <c r="I9" s="398" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>393</v>
@@ -8416,19 +8410,19 @@
         <v>394</v>
       </c>
       <c r="M9" s="411" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="N9" s="291" t="s">
         <v>562</v>
       </c>
       <c r="O9" s="417" t="s">
-        <v>1026</v>
+        <v>789</v>
       </c>
       <c r="P9" s="418" t="s">
         <v>409</v>
       </c>
       <c r="Q9" s="411" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="R9" s="421" t="s">
         <v>395</v>
@@ -8450,7 +8444,7 @@
         <v>396</v>
       </c>
       <c r="Y9" s="439" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="Z9" s="440" t="s">
         <v>397</v>
@@ -8463,7 +8457,7 @@
       </c>
       <c r="AC9" s="459"/>
       <c r="AD9" s="448" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="AE9" s="458"/>
       <c r="AF9" s="460" t="s">
@@ -8566,31 +8560,31 @@
       <c r="G10" s="277"/>
       <c r="H10" s="400"/>
       <c r="I10" s="397" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>393</v>
       </c>
       <c r="K10" s="405" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="L10" s="406" t="s">
         <v>394</v>
       </c>
       <c r="M10" s="412" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="N10" s="279" t="s">
         <v>562</v>
       </c>
       <c r="O10" s="415" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="P10" s="416" t="s">
         <v>409</v>
       </c>
       <c r="Q10" s="412" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="R10" s="422" t="s">
         <v>395</v>
@@ -8602,7 +8596,7 @@
         <v>562</v>
       </c>
       <c r="U10" s="428" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="V10" s="424" t="s">
         <v>848</v>
@@ -8614,7 +8608,7 @@
         <v>396</v>
       </c>
       <c r="Y10" s="436" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="Z10" s="437" t="s">
         <v>397</v>
@@ -8629,7 +8623,7 @@
         <v>1025</v>
       </c>
       <c r="AD10" s="449" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="AE10" s="454"/>
       <c r="AF10" s="456" t="s">
@@ -8659,7 +8653,7 @@
         <v>407</v>
       </c>
       <c r="AP10" s="476" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="AQ10" s="277" t="s">
         <v>576</v>
@@ -8734,7 +8728,7 @@
         <v>394</v>
       </c>
       <c r="M11" s="409" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="N11" s="446" t="s">
         <v>562</v>
@@ -8746,7 +8740,7 @@
         <v>409</v>
       </c>
       <c r="Q11" s="409" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="R11" s="419" t="s">
         <v>395</v>
@@ -8758,7 +8752,7 @@
         <v>562</v>
       </c>
       <c r="U11" s="420" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="V11" s="442" t="s">
         <v>849</v>
@@ -8768,7 +8762,7 @@
         <v>396</v>
       </c>
       <c r="Y11" s="432" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="Z11" s="431" t="s">
         <v>397</v>
@@ -8781,7 +8775,7 @@
       </c>
       <c r="AC11" s="443"/>
       <c r="AD11" s="442" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="AE11" s="446"/>
       <c r="AF11" s="444" t="s">
@@ -8867,12 +8861,12 @@
         <v>391</v>
       </c>
       <c r="F12" s="410" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="G12" s="461"/>
       <c r="H12" s="472"/>
       <c r="I12" s="409" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="J12" s="43" t="s">
         <v>393</v>
@@ -8884,7 +8878,7 @@
         <v>394</v>
       </c>
       <c r="M12" s="409" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="N12" s="446" t="s">
         <v>562</v>
@@ -8896,7 +8890,7 @@
         <v>409</v>
       </c>
       <c r="Q12" s="409" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="R12" s="419" t="s">
         <v>586</v>
@@ -8908,19 +8902,19 @@
         <v>562</v>
       </c>
       <c r="U12" s="420" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="V12" s="90" t="s">
         <v>850</v>
       </c>
       <c r="W12" s="419" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="X12" s="87" t="s">
         <v>396</v>
       </c>
       <c r="Y12" s="432" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="Z12" s="430" t="s">
         <v>397</v>
@@ -8935,7 +8929,7 @@
         <v>570</v>
       </c>
       <c r="AD12" s="442" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="AE12" s="446"/>
       <c r="AF12" s="101" t="s">
@@ -9031,7 +9025,7 @@
       </c>
       <c r="H13" s="472"/>
       <c r="I13" s="409" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="J13" s="43" t="s">
         <v>393</v>
@@ -9043,7 +9037,7 @@
         <v>394</v>
       </c>
       <c r="M13" s="409" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="N13" s="446" t="s">
         <v>562</v>
@@ -9055,7 +9049,7 @@
         <v>409</v>
       </c>
       <c r="Q13" s="409" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="R13" s="419" t="s">
         <v>587</v>
@@ -9067,7 +9061,7 @@
         <v>562</v>
       </c>
       <c r="U13" s="420" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="V13" s="90" t="s">
         <v>851</v>
@@ -9079,7 +9073,7 @@
         <v>396</v>
       </c>
       <c r="Y13" s="432" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="Z13" s="430" t="s">
         <v>397</v>
@@ -9094,7 +9088,7 @@
         <v>591</v>
       </c>
       <c r="AD13" s="442" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="AE13" s="358"/>
       <c r="AF13" s="101" t="s">
@@ -9187,12 +9181,12 @@
         <v>391</v>
       </c>
       <c r="F14" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G14" s="44"/>
       <c r="H14" s="45"/>
       <c r="I14" s="381" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="J14" s="43" t="s">
         <v>393</v>
@@ -9204,7 +9198,7 @@
         <v>394</v>
       </c>
       <c r="M14" s="409" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="N14" s="106" t="s">
         <v>562</v>
@@ -9216,7 +9210,7 @@
         <v>409</v>
       </c>
       <c r="Q14" s="409" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="R14" s="92" t="s">
         <v>603</v>
@@ -9228,7 +9222,7 @@
         <v>562</v>
       </c>
       <c r="U14" s="420" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="V14" s="90" t="s">
         <v>852</v>
@@ -9240,7 +9234,7 @@
         <v>905</v>
       </c>
       <c r="Y14" s="432" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="Z14" s="93" t="s">
         <v>397</v>
@@ -9255,7 +9249,7 @@
         <v>593</v>
       </c>
       <c r="AD14" s="380" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="AE14" s="106"/>
       <c r="AF14" s="101" t="s">
@@ -9347,12 +9341,12 @@
         <v>391</v>
       </c>
       <c r="F15" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G15" s="461"/>
       <c r="H15" s="472"/>
       <c r="I15" s="381" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="J15" s="43" t="s">
         <v>393</v>
@@ -9364,7 +9358,7 @@
         <v>394</v>
       </c>
       <c r="M15" s="409" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="N15" s="446" t="s">
         <v>562</v>
@@ -9376,7 +9370,7 @@
         <v>409</v>
       </c>
       <c r="Q15" s="409" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="R15" s="419" t="s">
         <v>605</v>
@@ -9388,7 +9382,7 @@
         <v>562</v>
       </c>
       <c r="U15" s="420" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="V15" s="90" t="s">
         <v>853</v>
@@ -9400,7 +9394,7 @@
         <v>396</v>
       </c>
       <c r="Y15" s="432" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="Z15" s="430" t="s">
         <v>397</v>
@@ -9415,7 +9409,7 @@
         <v>607</v>
       </c>
       <c r="AD15" s="442" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="AE15" s="446"/>
       <c r="AF15" s="101" t="s">
@@ -9504,7 +9498,7 @@
         <v>911</v>
       </c>
       <c r="F16" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G16" s="44"/>
       <c r="H16" s="45"/>
@@ -9517,7 +9511,7 @@
         <v>394</v>
       </c>
       <c r="M16" s="409" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="N16" s="106" t="s">
         <v>562</v>
@@ -9529,7 +9523,7 @@
         <v>409</v>
       </c>
       <c r="Q16" s="409" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="R16" s="419" t="s">
         <v>892</v>
@@ -9541,7 +9535,7 @@
         <v>562</v>
       </c>
       <c r="U16" s="420" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="V16" s="90" t="s">
         <v>893</v>
@@ -9551,7 +9545,7 @@
         <v>905</v>
       </c>
       <c r="Y16" s="432" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="Z16" s="93" t="s">
         <v>397</v>
@@ -9564,7 +9558,7 @@
       </c>
       <c r="AC16" s="100"/>
       <c r="AD16" s="380" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="AE16" s="106"/>
       <c r="AF16" s="101" t="s">
@@ -9653,12 +9647,12 @@
         <v>391</v>
       </c>
       <c r="F17" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G17" s="44"/>
       <c r="H17" s="45"/>
       <c r="I17" s="381" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="J17" s="43" t="s">
         <v>393</v>
@@ -9670,7 +9664,7 @@
         <v>394</v>
       </c>
       <c r="M17" s="409" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="N17" s="106" t="s">
         <v>562</v>
@@ -9682,7 +9676,7 @@
         <v>409</v>
       </c>
       <c r="Q17" s="409" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>902</v>
@@ -9694,7 +9688,7 @@
         <v>562</v>
       </c>
       <c r="U17" s="420" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="V17" s="90" t="s">
         <v>893</v>
@@ -9704,7 +9698,7 @@
         <v>904</v>
       </c>
       <c r="Y17" s="432" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="Z17" s="93" t="s">
         <v>397</v>
@@ -9719,7 +9713,7 @@
         <v>570</v>
       </c>
       <c r="AD17" s="380" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="AE17" s="106"/>
       <c r="AF17" s="101" t="s">
@@ -9806,12 +9800,12 @@
         <v>911</v>
       </c>
       <c r="F18" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G18" s="44"/>
       <c r="H18" s="45"/>
       <c r="I18" s="381" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="J18" s="43" t="s">
         <v>910</v>
@@ -9823,7 +9817,7 @@
         <v>918</v>
       </c>
       <c r="M18" s="409" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="N18" s="106" t="s">
         <v>562</v>
@@ -9835,7 +9829,7 @@
         <v>409</v>
       </c>
       <c r="Q18" s="409" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="R18" s="92" t="s">
         <v>603</v>
@@ -9847,7 +9841,7 @@
         <v>562</v>
       </c>
       <c r="U18" s="420" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="V18" s="90" t="s">
         <v>893</v>
@@ -9859,7 +9853,7 @@
         <v>905</v>
       </c>
       <c r="Y18" s="432" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="Z18" s="93" t="s">
         <v>397</v>
@@ -9874,7 +9868,7 @@
         <v>570</v>
       </c>
       <c r="AD18" s="380" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="AE18" s="106"/>
       <c r="AF18" s="101" t="s">
@@ -9961,12 +9955,12 @@
         <v>911</v>
       </c>
       <c r="F19" s="410" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G19" s="44"/>
       <c r="H19" s="45"/>
       <c r="I19" s="381" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="J19" s="43" t="s">
         <v>393</v>
@@ -9978,7 +9972,7 @@
         <v>918</v>
       </c>
       <c r="M19" s="409" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="N19" s="106" t="s">
         <v>562</v>
@@ -9990,7 +9984,7 @@
         <v>409</v>
       </c>
       <c r="Q19" s="409" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="R19" s="92" t="s">
         <v>603</v>
@@ -10014,7 +10008,7 @@
         <v>905</v>
       </c>
       <c r="Y19" s="432" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="Z19" s="93" t="s">
         <v>397</v>
@@ -10029,7 +10023,7 @@
         <v>570</v>
       </c>
       <c r="AD19" s="380" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="AE19" s="106"/>
       <c r="AF19" s="101" t="s">
@@ -10133,7 +10127,7 @@
         <v>918</v>
       </c>
       <c r="M20" s="409" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="N20" s="106" t="s">
         <v>562</v>
@@ -10145,7 +10139,7 @@
         <v>409</v>
       </c>
       <c r="Q20" s="409" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="R20" s="92" t="s">
         <v>931</v>
@@ -10157,7 +10151,7 @@
         <v>562</v>
       </c>
       <c r="U20" s="420" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="V20" s="90" t="s">
         <v>926</v>
@@ -10169,7 +10163,7 @@
         <v>396</v>
       </c>
       <c r="Y20" s="432" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="Z20" s="93" t="s">
         <v>397</v>
@@ -10184,7 +10178,7 @@
         <v>932</v>
       </c>
       <c r="AD20" s="380" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="AE20" s="106"/>
       <c r="AF20" s="101" t="s">
@@ -10269,18 +10263,18 @@
         <v>421</v>
       </c>
       <c r="D21" s="667" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E21" s="559" t="s">
         <v>391</v>
       </c>
       <c r="F21" s="586" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="G21" s="560"/>
       <c r="H21" s="561"/>
       <c r="I21" s="587" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="J21" s="562" t="s">
         <v>393</v>
@@ -10292,7 +10286,7 @@
         <v>918</v>
       </c>
       <c r="M21" s="564" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="N21" s="565" t="s">
         <v>562</v>
@@ -10304,7 +10298,7 @@
         <v>409</v>
       </c>
       <c r="Q21" s="564" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="R21" s="92" t="s">
         <v>934</v>
@@ -10316,7 +10310,7 @@
         <v>562</v>
       </c>
       <c r="U21" s="566" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="V21" s="559" t="s">
         <v>926</v>
@@ -10328,7 +10322,7 @@
         <v>396</v>
       </c>
       <c r="Y21" s="567" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="Z21" s="568" t="s">
         <v>397</v>
@@ -10343,7 +10337,7 @@
         <v>935</v>
       </c>
       <c r="AD21" s="572" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="AE21" s="565"/>
       <c r="AF21" s="573" t="s">
@@ -14510,7 +14504,7 @@
   <dimension ref="A1:GI134"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15263,7 +15257,7 @@
         <v>266</v>
       </c>
       <c r="M8" s="718" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="N8" s="644"/>
       <c r="O8" s="260" t="s">
@@ -15279,7 +15273,7 @@
         <v>270</v>
       </c>
       <c r="S8" s="274" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="T8" s="27"/>
       <c r="U8" s="27"/>
@@ -15324,7 +15318,7 @@
         <v>270</v>
       </c>
       <c r="M9" s="718" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="N9" s="645"/>
       <c r="O9" s="260" t="s">
@@ -15340,7 +15334,7 @@
         <v>345</v>
       </c>
       <c r="S9" s="274" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="T9" s="27"/>
       <c r="U9" s="27"/>
@@ -15385,7 +15379,7 @@
         <v>266</v>
       </c>
       <c r="M10" s="719" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="N10" s="647"/>
       <c r="O10" s="623" t="s">
@@ -15446,7 +15440,7 @@
         <v>345</v>
       </c>
       <c r="M11" s="719" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="N11" s="647"/>
       <c r="O11" s="623" t="s">
@@ -15756,7 +15750,7 @@
         <v>21</v>
       </c>
       <c r="P16" s="722" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="Q16" s="171">
         <v>415.69</v>
@@ -17223,7 +17217,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="382" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D8" s="262" t="s">
         <v>147</v>
@@ -17265,7 +17259,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="434" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D9" s="262" t="s">
         <v>148</v>
@@ -17307,7 +17301,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="523" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D10" s="524" t="s">
         <v>47</v>
@@ -17347,7 +17341,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="523" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D11" s="531" t="s">
         <v>50</v>
@@ -17387,7 +17381,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="383" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D12" s="318" t="s">
         <v>50</v>
@@ -17427,7 +17421,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="384" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D13" s="125" t="s">
         <v>147</v>
@@ -17467,7 +17461,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="679" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D14" s="680" t="s">
         <v>152</v>
@@ -17507,7 +17501,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="689" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D15" s="690" t="s">
         <v>150</v>

</xml_diff>